<commit_message>
fix gene names of datasets
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0428EDF9-42BE-8841-B4B6-0477E4F3FFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD4C354-8A0A-7E42-BB01-C3BC836C1F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="328">
   <si>
     <t>Genome Biology</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -325,11 +325,6 @@
   </si>
   <si>
     <t>GSE85755</t>
-  </si>
-  <si>
-    <t>Mus musculus
-Danio rerio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Single-cell sequencing reveals dissociation-induced gene expression in tissue subpopulations</t>
@@ -633,11 +628,6 @@
     <t>Thymus</t>
   </si>
   <si>
-    <t>CEL-seq
-SORT-seq</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>GSE86469</t>
   </si>
   <si>
@@ -735,11 +725,6 @@
   </si>
   <si>
     <t>Embryonic Stem Cells</t>
-  </si>
-  <si>
-    <t>Muscle Stem Cells
-Fin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GSE78779</t>
@@ -1169,6 +1154,14 @@
   </si>
   <si>
     <t>data101_stimulated-dendritic-cells-PIC_shalek.rds</t>
+  </si>
+  <si>
+    <t>Mus musculus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muscle Stem Cells</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1626,7 +1619,7 @@
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -1657,13 +1650,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1684,22 +1677,22 @@
         <v>20</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>6</v>
@@ -1713,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1763,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1804,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>10</v>
@@ -1819,13 +1812,13 @@
         <v>65</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="15">
         <v>2304</v>
       </c>
       <c r="I4" s="15">
-        <v>34408</v>
+        <v>34404</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>26</v>
@@ -1834,10 +1827,10 @@
         <v>12</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="34">
@@ -1845,22 +1838,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="15">
         <v>2304</v>
@@ -1875,10 +1868,10 @@
         <v>12</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="17">
@@ -1886,22 +1879,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H6" s="15">
         <v>6842</v>
@@ -1922,7 +1915,7 @@
         <v>18</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="17">
@@ -1930,22 +1923,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H7" s="15">
         <v>9149</v>
@@ -1966,10 +1959,10 @@
         <v>12</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="17">
@@ -1977,22 +1970,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H8" s="15">
         <v>4959</v>
@@ -2010,10 +2003,10 @@
         <v>12</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18">
@@ -2021,13 +2014,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>10</v>
@@ -2036,7 +2029,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9" s="15">
         <v>1920</v>
@@ -2051,19 +2044,19 @@
         <v>2</v>
       </c>
       <c r="N9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="P9" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R9" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17">
@@ -2071,22 +2064,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H10" s="15">
         <v>4057</v>
@@ -2104,10 +2097,10 @@
         <v>12</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17">
@@ -2115,7 +2108,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>9</v>
@@ -2156,22 +2149,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H12" s="15">
         <v>661</v>
@@ -2209,16 +2202,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>27</v>
@@ -2263,16 +2256,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>27</v>
@@ -2317,22 +2310,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H15" s="19">
         <v>1572</v>
@@ -2371,22 +2364,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H16" s="19">
         <v>4515</v>
@@ -2425,22 +2418,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H17" s="19">
         <v>2702</v>
@@ -2479,16 +2472,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>27</v>
@@ -2533,16 +2526,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>27</v>
@@ -2587,22 +2580,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" s="19">
         <v>1247</v>
@@ -2641,22 +2634,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H21" s="19">
         <v>10465</v>
@@ -2695,7 +2688,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>9</v>
@@ -2745,13 +2738,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>39</v>
@@ -2782,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="17">
@@ -2790,7 +2783,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>9</v>
@@ -2805,7 +2798,7 @@
         <v>27</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H24" s="15">
         <v>672</v>
@@ -2835,12 +2828,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="34">
+    <row r="25" spans="1:18" ht="17">
       <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>9</v>
@@ -2849,25 +2842,22 @@
         <v>83</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>163</v>
+        <v>67</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>84</v>
+        <v>326</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>193</v>
+        <v>327</v>
       </c>
       <c r="H25" s="15">
-        <v>1433</v>
+        <v>665</v>
       </c>
       <c r="I25" s="15">
-        <v>12635</v>
+        <v>13841</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="L25" s="7">
-        <v>2</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>12</v>
@@ -2876,7 +2866,7 @@
         <v>69</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="17">
@@ -2884,7 +2874,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>9</v>
@@ -2905,7 +2895,7 @@
         <v>3072</v>
       </c>
       <c r="I26" s="15">
-        <v>19140</v>
+        <v>19127</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>26</v>
@@ -2914,7 +2904,7 @@
         <v>28</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P26" s="7">
         <v>0.1</v>
@@ -2931,22 +2921,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H27" s="15">
         <v>44</v>
@@ -2961,7 +2951,7 @@
         <v>2</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O27" s="7">
         <v>1000000</v>
@@ -2981,7 +2971,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>9</v>
@@ -3014,16 +3004,16 @@
         <v>28</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q28" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3031,7 +3021,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>9</v>
@@ -3064,16 +3054,16 @@
         <v>28</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q29" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R29" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3081,7 +3071,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>9</v>
@@ -3114,16 +3104,16 @@
         <v>28</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R30" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3131,7 +3121,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>9</v>
@@ -3164,16 +3154,16 @@
         <v>28</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q31" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R31" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3181,7 +3171,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>9</v>
@@ -3214,16 +3204,16 @@
         <v>28</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R32" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3231,7 +3221,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>9</v>
@@ -3264,16 +3254,16 @@
         <v>28</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3281,13 +3271,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>25</v>
@@ -3296,13 +3286,13 @@
         <v>65</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H34" s="18">
         <v>2880</v>
       </c>
       <c r="I34" s="18">
-        <v>41289</v>
+        <v>41287</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>26</v>
@@ -3316,10 +3306,10 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R34" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3327,22 +3317,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H35" s="18">
         <v>2880</v>
@@ -3362,10 +3352,10 @@
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
       <c r="Q35" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17">
@@ -3373,7 +3363,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>9</v>
@@ -3414,7 +3404,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>9</v>
@@ -3455,7 +3445,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>9</v>
@@ -3496,7 +3486,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>9</v>
@@ -3537,7 +3527,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>9</v>
@@ -3578,7 +3568,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>58</v>
@@ -3590,10 +3580,10 @@
         <v>38</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H41" s="15">
         <v>5952</v>
@@ -3622,7 +3612,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>58</v>
@@ -3634,10 +3624,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42" s="15">
         <v>1101</v>
@@ -3666,7 +3656,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>58</v>
@@ -3681,7 +3671,7 @@
         <v>65</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H43" s="15">
         <v>1192</v>
@@ -3716,7 +3706,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>9</v>
@@ -3757,7 +3747,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>9</v>
@@ -3798,7 +3788,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>9</v>
@@ -3813,7 +3803,7 @@
         <v>27</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H46" s="15">
         <v>3005</v>
@@ -3825,7 +3815,7 @@
         <v>26</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
@@ -3841,13 +3831,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>39</v>
@@ -3856,7 +3846,7 @@
         <v>27</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H47" s="15">
         <v>186</v>
@@ -3876,10 +3866,10 @@
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R47" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="R47" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="17">
@@ -3887,13 +3877,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>39</v>
@@ -3902,7 +3892,7 @@
         <v>27</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H48" s="15">
         <v>346</v>
@@ -3922,10 +3912,10 @@
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R48" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="R48" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="17">
@@ -3933,13 +3923,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>39</v>
@@ -3948,7 +3938,7 @@
         <v>27</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H49" s="15">
         <v>278</v>
@@ -3968,10 +3958,10 @@
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R49" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="R49" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="17">
@@ -3979,13 +3969,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>39</v>
@@ -3994,7 +3984,7 @@
         <v>27</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H50" s="15">
         <v>444</v>
@@ -4014,10 +4004,10 @@
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
       <c r="Q50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R50" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="R50" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="17">
@@ -4025,13 +4015,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>39</v>
@@ -4040,7 +4030,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H51" s="15">
         <v>312</v>
@@ -4060,10 +4050,10 @@
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
       <c r="Q51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R51" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="R51" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="17">
@@ -4071,13 +4061,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>52</v>
@@ -4112,7 +4102,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>9</v>
@@ -4127,7 +4117,7 @@
         <v>27</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H53" s="15">
         <v>1234</v>
@@ -4153,7 +4143,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>9</v>
@@ -4168,7 +4158,7 @@
         <v>27</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H54" s="15">
         <v>4403</v>
@@ -4194,7 +4184,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>9</v>
@@ -4235,7 +4225,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>9</v>
@@ -4276,22 +4266,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H57" s="15">
         <v>3108</v>
@@ -4309,10 +4299,10 @@
         <v>29</v>
       </c>
       <c r="Q57" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="R57" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="17">
@@ -4320,22 +4310,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H58" s="15">
         <v>5013</v>
@@ -4353,10 +4343,10 @@
         <v>29</v>
       </c>
       <c r="Q58" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="R58" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="17">
@@ -4364,22 +4354,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H59" s="15">
         <v>2874</v>
@@ -4397,10 +4387,10 @@
         <v>29</v>
       </c>
       <c r="Q59" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="R59" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="17">
@@ -4408,22 +4398,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H60" s="15">
         <v>5773</v>
@@ -4441,10 +4431,10 @@
         <v>12</v>
       </c>
       <c r="Q60" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="R60" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="17">
@@ -4452,22 +4442,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H61" s="15">
         <v>9966</v>
@@ -4488,10 +4478,10 @@
         <v>12</v>
       </c>
       <c r="Q61" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="R61" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="17">
@@ -4499,13 +4489,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>38</v>
@@ -4514,7 +4504,7 @@
         <v>65</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H62" s="15">
         <v>4582</v>
@@ -4535,7 +4525,7 @@
         <v>7</v>
       </c>
       <c r="R62" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="17">
@@ -4543,13 +4533,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>38</v>
@@ -4558,7 +4548,7 @@
         <v>65</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H63" s="15">
         <v>2882</v>
@@ -4579,7 +4569,7 @@
         <v>7</v>
       </c>
       <c r="R63" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="17">
@@ -4587,13 +4577,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>37</v>
@@ -4602,7 +4592,7 @@
         <v>65</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H64" s="15">
         <v>1599</v>
@@ -4620,10 +4610,10 @@
         <v>12</v>
       </c>
       <c r="Q64" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R64" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="17">
@@ -4631,13 +4621,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>38</v>
@@ -4646,7 +4636,7 @@
         <v>27</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H65" s="15">
         <v>12249</v>
@@ -4664,10 +4654,10 @@
         <v>12</v>
       </c>
       <c r="Q65" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R65" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="17">
@@ -4675,13 +4665,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>13</v>
@@ -4690,7 +4680,7 @@
         <v>27</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H66" s="15">
         <v>160</v>
@@ -4711,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="R66" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="17">
@@ -4719,13 +4709,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>13</v>
@@ -4734,7 +4724,7 @@
         <v>27</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H67" s="15">
         <v>192</v>
@@ -4755,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="R67" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="17">
@@ -4763,13 +4753,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>13</v>
@@ -4778,7 +4768,7 @@
         <v>27</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H68" s="15">
         <v>156</v>
@@ -4799,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="R68" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="17">
@@ -4807,13 +4797,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>13</v>
@@ -4822,7 +4812,7 @@
         <v>27</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H69" s="15">
         <v>153</v>
@@ -4843,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="R69" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="17">
@@ -4851,13 +4841,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>13</v>
@@ -4866,7 +4856,7 @@
         <v>27</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H70" s="15">
         <v>151</v>
@@ -4887,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="R70" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="17">
@@ -4895,13 +4885,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>13</v>
@@ -4910,7 +4900,7 @@
         <v>27</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H71" s="15">
         <v>132</v>
@@ -4931,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="R71" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="17">
@@ -4939,13 +4929,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>13</v>
@@ -4954,7 +4944,7 @@
         <v>27</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H72" s="15">
         <v>124</v>
@@ -4972,10 +4962,10 @@
         <v>12</v>
       </c>
       <c r="Q72" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R72" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="17">
@@ -4983,13 +4973,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>13</v>
@@ -4998,7 +4988,7 @@
         <v>27</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H73" s="15">
         <v>147</v>
@@ -5016,10 +5006,10 @@
         <v>12</v>
       </c>
       <c r="Q73" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R73" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="17">
@@ -5027,13 +5017,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>13</v>
@@ -5042,7 +5032,7 @@
         <v>27</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H74" s="15">
         <v>106</v>
@@ -5060,10 +5050,10 @@
         <v>12</v>
       </c>
       <c r="Q74" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R74" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="17">
@@ -5071,13 +5061,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>10</v>
@@ -5104,10 +5094,10 @@
         <v>12</v>
       </c>
       <c r="Q75" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R75" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="17">
@@ -5115,13 +5105,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>10</v>
@@ -5148,10 +5138,10 @@
         <v>12</v>
       </c>
       <c r="Q76" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R76" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="17">
@@ -5159,13 +5149,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>10</v>
@@ -5192,10 +5182,10 @@
         <v>12</v>
       </c>
       <c r="Q77" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R77" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="17">
@@ -5203,13 +5193,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>10</v>
@@ -5236,10 +5226,10 @@
         <v>12</v>
       </c>
       <c r="Q78" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R78" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="17">
@@ -5247,13 +5237,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>10</v>
@@ -5280,10 +5270,10 @@
         <v>12</v>
       </c>
       <c r="Q79" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R79" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="17">
@@ -5291,22 +5281,22 @@
         <v>79</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H80" s="15">
         <v>873</v>
@@ -5324,10 +5314,10 @@
         <v>29</v>
       </c>
       <c r="Q80" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R80" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="R80" s="7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="17">
@@ -5335,22 +5325,22 @@
         <v>80</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H81" s="15">
         <v>493</v>
@@ -5368,10 +5358,10 @@
         <v>29</v>
       </c>
       <c r="Q81" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R81" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="R81" s="7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="17">
@@ -5379,13 +5369,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>39</v>
@@ -5394,7 +5384,7 @@
         <v>27</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H82" s="15">
         <v>264</v>
@@ -5409,19 +5399,19 @@
         <v>3</v>
       </c>
       <c r="N82" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O82" s="7">
         <v>100</v>
       </c>
       <c r="P82" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q82" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R82" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="17">
@@ -5429,13 +5419,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>25</v>
@@ -5444,7 +5434,7 @@
         <v>14</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H83" s="15">
         <v>154</v>
@@ -5465,7 +5455,7 @@
         <v>69</v>
       </c>
       <c r="R83" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="17">
@@ -5473,13 +5463,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>25</v>
@@ -5488,7 +5478,7 @@
         <v>14</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H84" s="15">
         <v>155</v>
@@ -5509,7 +5499,7 @@
         <v>69</v>
       </c>
       <c r="R84" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="17">
@@ -5517,13 +5507,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>25</v>
@@ -5532,7 +5522,7 @@
         <v>14</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H85" s="15">
         <v>163</v>
@@ -5553,7 +5543,7 @@
         <v>69</v>
       </c>
       <c r="R85" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="17">
@@ -5561,13 +5551,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E86" s="7" t="s">
         <v>25</v>
@@ -5576,7 +5566,7 @@
         <v>14</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H86" s="15">
         <v>162</v>
@@ -5597,7 +5587,7 @@
         <v>69</v>
       </c>
       <c r="R86" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:18" ht="17">
@@ -5605,13 +5595,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>39</v>
@@ -5638,10 +5628,10 @@
         <v>29</v>
       </c>
       <c r="Q87" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R87" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="17">
@@ -5649,13 +5639,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>17</v>
@@ -5664,7 +5654,7 @@
         <v>14</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H88" s="15">
         <v>666</v>
@@ -5685,7 +5675,7 @@
         <v>73</v>
       </c>
       <c r="R88" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="17">
@@ -5693,13 +5683,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>17</v>
@@ -5708,7 +5698,7 @@
         <v>14</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H89" s="15">
         <v>649</v>
@@ -5729,7 +5719,7 @@
         <v>73</v>
       </c>
       <c r="R89" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="17">
@@ -5737,13 +5727,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>39</v>
@@ -5752,7 +5742,7 @@
         <v>27</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H90" s="15">
         <v>316</v>
@@ -5773,7 +5763,7 @@
         <v>76</v>
       </c>
       <c r="R90" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="17">
@@ -5781,13 +5771,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>39</v>
@@ -5796,7 +5786,7 @@
         <v>14</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H91" s="15">
         <v>1289</v>
@@ -5811,19 +5801,19 @@
         <v>5</v>
       </c>
       <c r="N91" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O91" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O91" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="P91" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q91" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R91" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="17">
@@ -5831,13 +5821,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>17</v>
@@ -5846,7 +5836,7 @@
         <v>27</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H92" s="15">
         <v>60</v>
@@ -5864,10 +5854,10 @@
         <v>29</v>
       </c>
       <c r="Q92" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R92" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="17">
@@ -5875,13 +5865,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>39</v>
@@ -5890,7 +5880,7 @@
         <v>14</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H93" s="15">
         <v>504</v>
@@ -5908,10 +5898,10 @@
         <v>29</v>
       </c>
       <c r="Q93" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R93" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:18" ht="17">
@@ -5919,13 +5909,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>39</v>
@@ -5934,7 +5924,7 @@
         <v>14</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H94" s="15">
         <v>290</v>
@@ -5952,10 +5942,10 @@
         <v>29</v>
       </c>
       <c r="Q94" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R94" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="17">
@@ -5963,13 +5953,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>39</v>
@@ -5978,7 +5968,7 @@
         <v>27</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H95" s="15">
         <v>197</v>
@@ -5996,10 +5986,10 @@
         <v>29</v>
       </c>
       <c r="Q95" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R95" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="17">
@@ -6007,13 +5997,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>17</v>
@@ -6022,7 +6012,7 @@
         <v>27</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H96" s="15">
         <v>322</v>
@@ -6037,7 +6027,7 @@
         <v>6</v>
       </c>
       <c r="N96" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O96" s="8">
         <v>500000</v>
@@ -6049,7 +6039,7 @@
         <v>19</v>
       </c>
       <c r="R96" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:18" ht="17">
@@ -6057,13 +6047,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>17</v>
@@ -6072,7 +6062,7 @@
         <v>27</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H97" s="15">
         <v>562</v>
@@ -6087,7 +6077,7 @@
         <v>7</v>
       </c>
       <c r="N97" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O97" s="8">
         <v>500000</v>
@@ -6099,7 +6089,7 @@
         <v>19</v>
       </c>
       <c r="R97" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="17">
@@ -6107,13 +6097,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>17</v>
@@ -6122,7 +6112,7 @@
         <v>14</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H98" s="15">
         <v>455</v>
@@ -6140,10 +6130,10 @@
         <v>29</v>
       </c>
       <c r="Q98" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R98" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="17">
@@ -6151,13 +6141,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>17</v>
@@ -6166,7 +6156,7 @@
         <v>14</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H99" s="15">
         <v>192</v>
@@ -6181,19 +6171,19 @@
         <v>4</v>
       </c>
       <c r="N99" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O99" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O99" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="P99" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q99" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R99" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:18" ht="17">
@@ -6201,22 +6191,22 @@
         <v>99</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H100" s="15">
         <v>540</v>
@@ -6237,7 +6227,7 @@
         <v>76</v>
       </c>
       <c r="R100" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:18" ht="17">
@@ -6245,22 +6235,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H101" s="15">
         <v>407</v>
@@ -6281,7 +6271,7 @@
         <v>76</v>
       </c>
       <c r="R101" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:18" ht="17">
@@ -6289,22 +6279,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H102" s="15">
         <v>433</v>
@@ -6325,7 +6315,7 @@
         <v>76</v>
       </c>
       <c r="R102" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:18">

</xml_diff>

<commit_message>
fix gene names of GSE87038 datasets
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD4C354-8A0A-7E42-BB01-C3BC836C1F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35A45C-AF9D-8A45-BFFA-36068A0C164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1617,9 +1617,9 @@
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
code in Splatter package methods and reference data properties
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35A45C-AF9D-8A45-BFFA-36068A0C164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD73F76-3940-D840-970D-F860E55C8BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="11" r:id="rId1"/>
@@ -1617,9 +1617,9 @@
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="H74" sqref="H74"/>
+      <selection pane="bottomLeft" activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
remove cells in all genes in data35 and data38
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD73F76-3940-D840-970D-F860E55C8BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CED1638-26F6-214F-97AD-05D6417872E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,7 +1619,7 @@
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="M49" sqref="M49"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -3381,7 +3381,7 @@
         <v>35</v>
       </c>
       <c r="H36" s="15">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="I36" s="15">
         <v>24973</v>
@@ -3504,7 +3504,7 @@
         <v>35</v>
       </c>
       <c r="H39" s="15">
-        <v>2000</v>
+        <v>1996</v>
       </c>
       <c r="I39" s="15">
         <v>23342</v>

</xml_diff>

<commit_message>
fix datasets summary xlsx
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CED1638-26F6-214F-97AD-05D6417872E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7784BAC8-BD49-5848-8C80-F21940BAF0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,7 +1619,7 @@
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add scalability and fix datasets information
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED2B55-FA80-644F-A343-B6A4738388A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF21F8BC-EC46-C246-A7E3-98A0A737844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="11" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="331">
   <si>
     <t>Genome Biology</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>Droplet barcoding for single-cell transcriptomics applied to embryonic stem cells</t>
-  </si>
-  <si>
-    <t>CEL-Seq2: sensitive highly-multiplexed single-cell RNA-Seq</t>
   </si>
   <si>
     <t>Cell Stem Cell</t>
@@ -1161,6 +1158,24 @@
   </si>
   <si>
     <t>Muscle Stem Cells</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single-cell transcriptomics of 20 mouse organs creates a Tabula Muris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>500000
+(2500000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEL-Seq2: sensitive highly-multiplexed single-cell RNA-Seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50000
+(40000000)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1252,7 +1267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1318,6 +1333,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1616,10 +1634,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -1650,13 +1668,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1677,22 +1695,22 @@
         <v>20</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>6</v>
@@ -1701,12 +1719,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17">
+    <row r="2" spans="1:18" ht="34">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1738,8 +1756,8 @@
       <c r="N2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="8">
-        <v>50000</v>
+      <c r="O2" s="23" t="s">
+        <v>330</v>
       </c>
       <c r="P2" s="7">
         <v>0.01</v>
@@ -1756,13 +1774,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>10</v>
@@ -1771,7 +1789,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" s="15">
         <v>10368</v>
@@ -1789,7 +1807,7 @@
         <v>7</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="34">
@@ -1797,13 +1815,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>10</v>
@@ -1812,7 +1830,7 @@
         <v>65</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="15">
         <v>2304</v>
@@ -1827,10 +1845,10 @@
         <v>12</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="34">
@@ -1838,22 +1856,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="15">
         <v>2304</v>
@@ -1868,10 +1886,10 @@
         <v>12</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="17">
@@ -1879,22 +1897,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="15">
         <v>6842</v>
@@ -1915,7 +1933,7 @@
         <v>18</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="17">
@@ -1923,22 +1941,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H7" s="15">
         <v>9149</v>
@@ -1959,10 +1977,10 @@
         <v>12</v>
       </c>
       <c r="Q7" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="R7" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="17">
@@ -1970,22 +1988,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>195</v>
-      </c>
       <c r="F8" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>207</v>
       </c>
       <c r="H8" s="15">
         <v>4959</v>
@@ -2003,10 +2021,10 @@
         <v>12</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18">
@@ -2014,13 +2032,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>10</v>
@@ -2029,7 +2047,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="15">
         <v>1920</v>
@@ -2044,19 +2062,19 @@
         <v>2</v>
       </c>
       <c r="N9" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="P9" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R9" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17">
@@ -2064,22 +2082,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H10" s="15">
         <v>4057</v>
@@ -2097,10 +2115,10 @@
         <v>12</v>
       </c>
       <c r="Q10" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="R10" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17">
@@ -2108,7 +2126,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>9</v>
@@ -2149,22 +2167,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H12" s="15">
         <v>661</v>
@@ -2194,7 +2212,7 @@
         <v>36</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>55</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="3" customFormat="1" ht="34">
@@ -2202,16 +2220,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>27</v>
@@ -2256,16 +2274,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>27</v>
@@ -2310,22 +2328,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="19">
         <v>1572</v>
@@ -2364,22 +2382,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H16" s="19">
         <v>4515</v>
@@ -2418,22 +2436,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H17" s="19">
         <v>2702</v>
@@ -2472,16 +2490,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>27</v>
@@ -2526,16 +2544,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>27</v>
@@ -2580,22 +2598,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H20" s="19">
         <v>1247</v>
@@ -2634,22 +2652,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H21" s="19">
         <v>10465</v>
@@ -2683,12 +2701,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="17">
+    <row r="22" spans="1:18" ht="34">
       <c r="A22" s="10">
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>9</v>
@@ -2703,7 +2721,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H22" s="15">
         <v>160</v>
@@ -2720,8 +2738,8 @@
       <c r="N22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O22" s="8">
-        <v>500000</v>
+      <c r="O22" s="23" t="s">
+        <v>328</v>
       </c>
       <c r="P22" s="7">
         <v>1</v>
@@ -2738,13 +2756,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>39</v>
@@ -2775,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="17">
@@ -2783,13 +2801,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>67</v>
@@ -2798,7 +2816,7 @@
         <v>27</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H24" s="15">
         <v>672</v>
@@ -2822,7 +2840,7 @@
         <v>0.03</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R24" s="7" t="s">
         <v>57</v>
@@ -2833,22 +2851,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>326</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>327</v>
       </c>
       <c r="H25" s="15">
         <v>665</v>
@@ -2866,7 +2884,7 @@
         <v>69</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="17">
@@ -2874,7 +2892,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>9</v>
@@ -2904,7 +2922,7 @@
         <v>28</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P26" s="7">
         <v>0.1</v>
@@ -2921,22 +2939,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H27" s="15">
         <v>44</v>
@@ -2951,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O27" s="7">
         <v>1000000</v>
@@ -2963,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="R27" s="7" t="s">
-        <v>72</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="2" customFormat="1" ht="17">
@@ -2971,7 +2989,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>9</v>
@@ -3004,16 +3022,16 @@
         <v>28</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q28" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3021,7 +3039,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>9</v>
@@ -3054,16 +3072,16 @@
         <v>28</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q29" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R29" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3071,7 +3089,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>9</v>
@@ -3104,16 +3122,16 @@
         <v>28</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R30" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3121,7 +3139,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>9</v>
@@ -3154,16 +3172,16 @@
         <v>28</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q31" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R31" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3171,7 +3189,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>9</v>
@@ -3204,16 +3222,16 @@
         <v>28</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R32" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3221,7 +3239,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>9</v>
@@ -3254,16 +3272,16 @@
         <v>28</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>69</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3271,13 +3289,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>25</v>
@@ -3286,7 +3304,7 @@
         <v>65</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H34" s="18">
         <v>2880</v>
@@ -3306,10 +3324,10 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R34" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="4" customFormat="1" ht="17">
@@ -3317,22 +3335,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H35" s="18">
         <v>2880</v>
@@ -3352,10 +3370,10 @@
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
       <c r="Q35" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17">
@@ -3363,7 +3381,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>9</v>
@@ -3404,7 +3422,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>9</v>
@@ -3445,7 +3463,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>9</v>
@@ -3486,7 +3504,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>9</v>
@@ -3527,7 +3545,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>9</v>
@@ -3568,7 +3586,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>58</v>
@@ -3580,10 +3598,10 @@
         <v>38</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H41" s="15">
         <v>5952</v>
@@ -3612,7 +3630,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>58</v>
@@ -3624,10 +3642,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H42" s="15">
         <v>1101</v>
@@ -3656,7 +3674,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>58</v>
@@ -3671,7 +3689,7 @@
         <v>65</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H43" s="15">
         <v>1192</v>
@@ -3706,13 +3724,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>39</v>
@@ -3736,10 +3754,10 @@
         <v>12</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R44" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="17">
@@ -3747,7 +3765,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>9</v>
@@ -3788,7 +3806,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>9</v>
@@ -3803,7 +3821,7 @@
         <v>27</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H46" s="15">
         <v>3005</v>
@@ -3815,7 +3833,7 @@
         <v>26</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
@@ -3831,13 +3849,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>39</v>
@@ -3846,7 +3864,7 @@
         <v>27</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H47" s="15">
         <v>186</v>
@@ -3866,10 +3884,10 @@
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R47" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="R47" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="17">
@@ -3877,13 +3895,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>39</v>
@@ -3892,7 +3910,7 @@
         <v>27</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H48" s="15">
         <v>346</v>
@@ -3912,10 +3930,10 @@
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R48" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="R48" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="17">
@@ -3923,13 +3941,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>39</v>
@@ -3938,7 +3956,7 @@
         <v>27</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H49" s="15">
         <v>278</v>
@@ -3958,10 +3976,10 @@
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R49" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="R49" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="17">
@@ -3969,13 +3987,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>39</v>
@@ -3984,7 +4002,7 @@
         <v>27</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H50" s="15">
         <v>444</v>
@@ -4004,10 +4022,10 @@
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
       <c r="Q50" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R50" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="R50" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="17">
@@ -4015,13 +4033,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>39</v>
@@ -4030,7 +4048,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H51" s="15">
         <v>312</v>
@@ -4050,10 +4068,10 @@
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
       <c r="Q51" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R51" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="R51" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="17">
@@ -4061,13 +4079,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>52</v>
@@ -4102,7 +4120,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>9</v>
@@ -4117,7 +4135,7 @@
         <v>27</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H53" s="15">
         <v>1234</v>
@@ -4143,7 +4161,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>9</v>
@@ -4158,7 +4176,7 @@
         <v>27</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H54" s="15">
         <v>4403</v>
@@ -4184,7 +4202,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>9</v>
@@ -4199,7 +4217,7 @@
         <v>27</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H55" s="15">
         <v>541</v>
@@ -4225,7 +4243,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>9</v>
@@ -4240,7 +4258,7 @@
         <v>27</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H56" s="15">
         <v>5345</v>
@@ -4266,22 +4284,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H57" s="15">
         <v>3108</v>
@@ -4299,10 +4317,10 @@
         <v>29</v>
       </c>
       <c r="Q57" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R57" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="17">
@@ -4310,22 +4328,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H58" s="15">
         <v>5013</v>
@@ -4343,10 +4361,10 @@
         <v>29</v>
       </c>
       <c r="Q58" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R58" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="17">
@@ -4354,22 +4372,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H59" s="15">
         <v>2874</v>
@@ -4387,10 +4405,10 @@
         <v>29</v>
       </c>
       <c r="Q59" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R59" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="17">
@@ -4398,22 +4416,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H60" s="15">
         <v>5773</v>
@@ -4431,10 +4449,10 @@
         <v>12</v>
       </c>
       <c r="Q60" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R60" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="17">
@@ -4442,22 +4460,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H61" s="15">
         <v>9966</v>
@@ -4478,10 +4496,10 @@
         <v>12</v>
       </c>
       <c r="Q61" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R61" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="17">
@@ -4489,13 +4507,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>38</v>
@@ -4504,7 +4522,7 @@
         <v>65</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H62" s="15">
         <v>4582</v>
@@ -4525,7 +4543,7 @@
         <v>7</v>
       </c>
       <c r="R62" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="17">
@@ -4533,13 +4551,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>38</v>
@@ -4548,7 +4566,7 @@
         <v>65</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H63" s="15">
         <v>2882</v>
@@ -4569,7 +4587,7 @@
         <v>7</v>
       </c>
       <c r="R63" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="17">
@@ -4577,13 +4595,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>37</v>
@@ -4592,7 +4610,7 @@
         <v>65</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H64" s="15">
         <v>1599</v>
@@ -4610,10 +4628,10 @@
         <v>12</v>
       </c>
       <c r="Q64" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R64" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="17">
@@ -4621,13 +4639,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>38</v>
@@ -4636,7 +4654,7 @@
         <v>27</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H65" s="15">
         <v>12249</v>
@@ -4654,10 +4672,10 @@
         <v>12</v>
       </c>
       <c r="Q65" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R65" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="17">
@@ -4665,13 +4683,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>13</v>
@@ -4680,7 +4698,7 @@
         <v>27</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H66" s="15">
         <v>160</v>
@@ -4701,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="R66" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="17">
@@ -4709,13 +4727,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>13</v>
@@ -4724,7 +4742,7 @@
         <v>27</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H67" s="15">
         <v>192</v>
@@ -4745,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="R67" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="17">
@@ -4753,13 +4771,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>13</v>
@@ -4768,7 +4786,7 @@
         <v>27</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H68" s="15">
         <v>156</v>
@@ -4789,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="R68" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="17">
@@ -4797,13 +4815,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>13</v>
@@ -4812,7 +4830,7 @@
         <v>27</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H69" s="15">
         <v>153</v>
@@ -4833,7 +4851,7 @@
         <v>0</v>
       </c>
       <c r="R69" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="17">
@@ -4841,13 +4859,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>13</v>
@@ -4856,7 +4874,7 @@
         <v>27</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H70" s="15">
         <v>151</v>
@@ -4877,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="R70" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="17">
@@ -4885,13 +4903,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>13</v>
@@ -4900,7 +4918,7 @@
         <v>27</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H71" s="15">
         <v>132</v>
@@ -4921,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="R71" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="17">
@@ -4929,13 +4947,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>13</v>
@@ -4944,7 +4962,7 @@
         <v>27</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H72" s="15">
         <v>124</v>
@@ -4962,10 +4980,10 @@
         <v>12</v>
       </c>
       <c r="Q72" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R72" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="17">
@@ -4973,13 +4991,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>13</v>
@@ -4988,7 +5006,7 @@
         <v>27</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H73" s="15">
         <v>147</v>
@@ -5006,10 +5024,10 @@
         <v>12</v>
       </c>
       <c r="Q73" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R73" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="17">
@@ -5017,13 +5035,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>13</v>
@@ -5032,7 +5050,7 @@
         <v>27</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H74" s="15">
         <v>106</v>
@@ -5050,10 +5068,10 @@
         <v>12</v>
       </c>
       <c r="Q74" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R74" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="17">
@@ -5061,13 +5079,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>10</v>
@@ -5076,7 +5094,7 @@
         <v>27</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H75" s="15">
         <v>768</v>
@@ -5094,10 +5112,10 @@
         <v>12</v>
       </c>
       <c r="Q75" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R75" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="17">
@@ -5105,13 +5123,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>10</v>
@@ -5120,7 +5138,7 @@
         <v>27</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H76" s="15">
         <v>768</v>
@@ -5138,10 +5156,10 @@
         <v>12</v>
       </c>
       <c r="Q76" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R76" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="17">
@@ -5149,13 +5167,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>10</v>
@@ -5164,7 +5182,7 @@
         <v>27</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H77" s="15">
         <v>768</v>
@@ -5182,10 +5200,10 @@
         <v>12</v>
       </c>
       <c r="Q77" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R77" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="17">
@@ -5193,13 +5211,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>10</v>
@@ -5208,7 +5226,7 @@
         <v>27</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H78" s="15">
         <v>768</v>
@@ -5226,10 +5244,10 @@
         <v>12</v>
       </c>
       <c r="Q78" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R78" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="17">
@@ -5237,13 +5255,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>10</v>
@@ -5252,7 +5270,7 @@
         <v>27</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H79" s="15">
         <v>768</v>
@@ -5270,10 +5288,10 @@
         <v>12</v>
       </c>
       <c r="Q79" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R79" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="17">
@@ -5281,22 +5299,22 @@
         <v>79</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H80" s="15">
         <v>873</v>
@@ -5314,10 +5332,10 @@
         <v>29</v>
       </c>
       <c r="Q80" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="R80" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="R80" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="17">
@@ -5325,22 +5343,22 @@
         <v>80</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H81" s="15">
         <v>493</v>
@@ -5358,10 +5376,10 @@
         <v>29</v>
       </c>
       <c r="Q81" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="R81" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="R81" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="17">
@@ -5369,13 +5387,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>39</v>
@@ -5384,7 +5402,7 @@
         <v>27</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H82" s="15">
         <v>264</v>
@@ -5399,19 +5417,19 @@
         <v>3</v>
       </c>
       <c r="N82" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O82" s="7">
         <v>100</v>
       </c>
       <c r="P82" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q82" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R82" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="17">
@@ -5419,13 +5437,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>25</v>
@@ -5434,7 +5452,7 @@
         <v>14</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H83" s="15">
         <v>154</v>
@@ -5455,7 +5473,7 @@
         <v>69</v>
       </c>
       <c r="R83" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="17">
@@ -5463,13 +5481,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>25</v>
@@ -5478,7 +5496,7 @@
         <v>14</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H84" s="15">
         <v>155</v>
@@ -5499,7 +5517,7 @@
         <v>69</v>
       </c>
       <c r="R84" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="17">
@@ -5507,13 +5525,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>25</v>
@@ -5522,7 +5540,7 @@
         <v>14</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H85" s="15">
         <v>163</v>
@@ -5543,7 +5561,7 @@
         <v>69</v>
       </c>
       <c r="R85" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="17">
@@ -5551,13 +5569,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E86" s="7" t="s">
         <v>25</v>
@@ -5566,7 +5584,7 @@
         <v>14</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H86" s="15">
         <v>162</v>
@@ -5587,7 +5605,7 @@
         <v>69</v>
       </c>
       <c r="R86" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:18" ht="17">
@@ -5595,13 +5613,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>39</v>
@@ -5610,7 +5628,7 @@
         <v>27</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H87" s="15">
         <v>238</v>
@@ -5628,10 +5646,10 @@
         <v>29</v>
       </c>
       <c r="Q87" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R87" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="17">
@@ -5639,13 +5657,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>17</v>
@@ -5654,7 +5672,7 @@
         <v>14</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H88" s="15">
         <v>666</v>
@@ -5672,10 +5690,10 @@
         <v>29</v>
       </c>
       <c r="Q88" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R88" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="17">
@@ -5683,13 +5701,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>17</v>
@@ -5698,7 +5716,7 @@
         <v>14</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H89" s="15">
         <v>649</v>
@@ -5716,10 +5734,10 @@
         <v>29</v>
       </c>
       <c r="Q89" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R89" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="17">
@@ -5727,13 +5745,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>39</v>
@@ -5742,7 +5760,7 @@
         <v>27</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H90" s="15">
         <v>316</v>
@@ -5760,10 +5778,10 @@
         <v>29</v>
       </c>
       <c r="Q90" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R90" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="17">
@@ -5771,13 +5789,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>39</v>
@@ -5786,7 +5804,7 @@
         <v>14</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H91" s="15">
         <v>1289</v>
@@ -5801,19 +5819,19 @@
         <v>5</v>
       </c>
       <c r="N91" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O91" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="O91" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="P91" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q91" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R91" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="17">
@@ -5821,13 +5839,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>17</v>
@@ -5836,7 +5854,7 @@
         <v>27</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H92" s="15">
         <v>60</v>
@@ -5854,10 +5872,10 @@
         <v>29</v>
       </c>
       <c r="Q92" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R92" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="17">
@@ -5865,13 +5883,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>39</v>
@@ -5880,7 +5898,7 @@
         <v>14</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H93" s="15">
         <v>504</v>
@@ -5898,10 +5916,10 @@
         <v>29</v>
       </c>
       <c r="Q93" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R93" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:18" ht="17">
@@ -5909,13 +5927,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>39</v>
@@ -5924,7 +5942,7 @@
         <v>14</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H94" s="15">
         <v>290</v>
@@ -5942,10 +5960,10 @@
         <v>29</v>
       </c>
       <c r="Q94" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R94" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="17">
@@ -5953,13 +5971,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>39</v>
@@ -5968,7 +5986,7 @@
         <v>27</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H95" s="15">
         <v>197</v>
@@ -5986,10 +6004,10 @@
         <v>29</v>
       </c>
       <c r="Q95" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R95" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="17">
@@ -5997,13 +6015,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>17</v>
@@ -6012,7 +6030,7 @@
         <v>27</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H96" s="15">
         <v>322</v>
@@ -6027,7 +6045,7 @@
         <v>6</v>
       </c>
       <c r="N96" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O96" s="8">
         <v>500000</v>
@@ -6039,7 +6057,7 @@
         <v>19</v>
       </c>
       <c r="R96" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:18" ht="17">
@@ -6047,13 +6065,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>17</v>
@@ -6062,7 +6080,7 @@
         <v>27</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H97" s="15">
         <v>562</v>
@@ -6077,7 +6095,7 @@
         <v>7</v>
       </c>
       <c r="N97" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O97" s="8">
         <v>500000</v>
@@ -6089,7 +6107,7 @@
         <v>19</v>
       </c>
       <c r="R97" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="17">
@@ -6097,13 +6115,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>17</v>
@@ -6112,7 +6130,7 @@
         <v>14</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H98" s="15">
         <v>455</v>
@@ -6130,10 +6148,10 @@
         <v>29</v>
       </c>
       <c r="Q98" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R98" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="17">
@@ -6141,13 +6159,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>17</v>
@@ -6156,7 +6174,7 @@
         <v>14</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H99" s="15">
         <v>192</v>
@@ -6171,19 +6189,19 @@
         <v>4</v>
       </c>
       <c r="N99" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O99" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="O99" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="P99" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q99" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R99" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:18" ht="17">
@@ -6191,22 +6209,22 @@
         <v>99</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H100" s="15">
         <v>540</v>
@@ -6224,10 +6242,10 @@
         <v>29</v>
       </c>
       <c r="Q100" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R100" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" spans="1:18" ht="17">
@@ -6235,22 +6253,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H101" s="15">
         <v>407</v>
@@ -6268,10 +6286,10 @@
         <v>29</v>
       </c>
       <c r="Q101" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R101" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:18" ht="17">
@@ -6279,22 +6297,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H102" s="15">
         <v>433</v>
@@ -6312,10 +6330,10 @@
         <v>29</v>
       </c>
       <c r="Q102" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R102" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:18">

</xml_diff>

<commit_message>
add datasets and fix scalability
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1A4DB-0EE9-8141-BB64-A0E4DA03DE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F48C9C4-2E9A-2E4E-A307-7DD23311E7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="347">
   <si>
     <t>Genome Biology</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1219,6 +1219,25 @@
   <si>
     <t>data107_spatial_H1.rds</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data108_spatial_HDST1.rds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCP420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nature Methods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High-definition spatial transcriptomics for in situ tissue profiling</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1695,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:R125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -6642,90 +6661,142 @@
         <v>334</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" ht="17">
       <c r="A109" s="10">
         <v>108</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="H109" s="15">
+        <v>4137</v>
+      </c>
+      <c r="I109" s="15">
+        <v>18284</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K109" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="110" spans="1:18">
       <c r="A110" s="10">
         <v>109</v>
       </c>
+      <c r="B110" s="7"/>
     </row>
     <row r="111" spans="1:18">
       <c r="A111" s="10">
         <v>110</v>
       </c>
+      <c r="B111" s="7"/>
     </row>
     <row r="112" spans="1:18">
       <c r="A112" s="10">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" s="7"/>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113" s="10">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114" s="10">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114" s="7"/>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115" s="10">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115" s="7"/>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116" s="10">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116" s="7"/>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117" s="10">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117" s="7"/>
+    </row>
+    <row r="118" spans="1:2">
       <c r="A118" s="10">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118" s="7"/>
+    </row>
+    <row r="119" spans="1:2">
       <c r="A119" s="10">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119" s="7"/>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" s="10">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120" s="7"/>
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" s="10">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121" s="7"/>
+    </row>
+    <row r="122" spans="1:2">
       <c r="A122" s="10">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122" s="7"/>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123" s="10">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123" s="7"/>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124" s="10">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124" s="7"/>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125" s="10">
         <v>124</v>
       </c>
+      <c r="B125" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update data analysis and DEGs for scDD
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B0343-4961-2945-AC3C-B284430D1328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F18EEB-CF33-2E40-AD79-E0410B6A5672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="11" r:id="rId1"/>
@@ -2089,10 +2089,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B98:B108"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -9067,7 +9067,7 @@
         <v>214</v>
       </c>
       <c r="H146" s="15">
-        <v>17679</v>
+        <v>2863</v>
       </c>
       <c r="I146" s="15">
         <v>374</v>
@@ -9091,11 +9091,11 @@
         <v>405</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="17">
+    <row r="147" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A147" s="10">
         <v>146</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="7" t="s">
         <v>424</v>
       </c>
       <c r="D147" s="9" t="s">
@@ -9135,11 +9135,11 @@
         <v>408</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="17">
+    <row r="148" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A148" s="10">
         <v>147</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="7" t="s">
         <v>423</v>
       </c>
       <c r="D148" s="9" t="s">
@@ -9179,11 +9179,11 @@
         <v>408</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="17">
+    <row r="149" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A149" s="10">
         <v>148</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="7" t="s">
         <v>422</v>
       </c>
       <c r="D149" s="9" t="s">
@@ -9223,11 +9223,11 @@
         <v>408</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="17">
+    <row r="150" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A150" s="10">
         <v>149</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="7" t="s">
         <v>421</v>
       </c>
       <c r="D150" s="9" t="s">
@@ -9267,11 +9267,11 @@
         <v>408</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="17">
+    <row r="151" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A151" s="10">
         <v>150</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="7" t="s">
         <v>420</v>
       </c>
       <c r="D151" s="9" t="s">
@@ -9311,11 +9311,11 @@
         <v>417</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="17">
+    <row r="152" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A152" s="10">
         <v>151</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="7" t="s">
         <v>419</v>
       </c>
       <c r="D152" s="9" t="s">
@@ -9355,11 +9355,11 @@
         <v>417</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="17">
+    <row r="153" spans="1:19" s="7" customFormat="1" ht="17">
       <c r="A153" s="10">
         <v>152</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="7" t="s">
         <v>418</v>
       </c>
       <c r="D153" s="9" t="s">

</xml_diff>

<commit_message>
add micro values and fix methods codes errors
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2DF8DC-E0EA-6546-AB7C-894CBD73A1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC1A706-D011-6246-9414-1D25062BBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2089,10 +2089,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
data analysis and add gradient number
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC1A706-D011-6246-9414-1D25062BBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F545B42D-FF1E-4546-B735-4F50FC3FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2089,10 +2089,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add analytical codes and data
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F545B42D-FF1E-4546-B735-4F50FC3FB37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D79E92E-6C7C-1B40-A58C-5969F0A3DD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1378,9 +1378,6 @@
     <t>https://content.cruk.cam.ac.uk/jmlab/SpatialMouseAtlas2020/</t>
   </si>
   <si>
-    <t xml:space="preserve">seqFISH </t>
-  </si>
-  <si>
     <t xml:space="preserve">Gastrulation </t>
   </si>
   <si>
@@ -1628,6 +1625,10 @@
   </si>
   <si>
     <t>data116_spatial_PRAD.rds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqFISH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2090,9 +2091,9 @@
   <dimension ref="A1:S153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="C119" sqref="C119"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -4481,7 +4482,7 @@
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
       <c r="R47" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>94</v>
@@ -4530,7 +4531,7 @@
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
       <c r="R48" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S48" s="7" t="s">
         <v>94</v>
@@ -4579,7 +4580,7 @@
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
       <c r="R49" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S49" s="7" t="s">
         <v>94</v>
@@ -4628,7 +4629,7 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
       <c r="R50" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S50" s="7" t="s">
         <v>94</v>
@@ -4677,7 +4678,7 @@
       <c r="P51" s="11"/>
       <c r="Q51" s="11"/>
       <c r="R51" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S51" s="7" t="s">
         <v>94</v>
@@ -7139,7 +7140,7 @@
         <v>11</v>
       </c>
       <c r="R103" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S103" s="7" t="s">
         <v>332</v>
@@ -7186,7 +7187,7 @@
         <v>11</v>
       </c>
       <c r="R104" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S104" s="7" t="s">
         <v>332</v>
@@ -7233,7 +7234,7 @@
         <v>11</v>
       </c>
       <c r="R105" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S105" s="7" t="s">
         <v>332</v>
@@ -7280,7 +7281,7 @@
         <v>11</v>
       </c>
       <c r="R106" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S106" s="7" t="s">
         <v>332</v>
@@ -7327,7 +7328,7 @@
         <v>11</v>
       </c>
       <c r="R107" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S107" s="7" t="s">
         <v>332</v>
@@ -7374,7 +7375,7 @@
         <v>11</v>
       </c>
       <c r="R108" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S108" s="7" t="s">
         <v>332</v>
@@ -7761,7 +7762,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>193</v>
@@ -7802,7 +7803,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>193</v>
@@ -7843,7 +7844,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>193</v>
@@ -7884,7 +7885,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>193</v>
@@ -7966,7 +7967,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>193</v>
@@ -8007,7 +8008,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>193</v>
@@ -8048,7 +8049,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>371</v>
@@ -8095,7 +8096,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C125" s="9" t="s">
         <v>191</v>
@@ -8142,7 +8143,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>191</v>
@@ -8189,7 +8190,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>191</v>
@@ -8236,7 +8237,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>191</v>
@@ -8283,7 +8284,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>191</v>
@@ -8330,7 +8331,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>191</v>
@@ -8377,19 +8378,19 @@
         <v>130</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>385</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="F131" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H131" s="15">
         <v>1260</v>
@@ -8413,7 +8414,7 @@
         <v>86</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="132" spans="1:19" ht="17">
@@ -8421,19 +8422,19 @@
         <v>131</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>385</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H132" s="15">
         <v>3704</v>
@@ -8457,7 +8458,7 @@
         <v>86</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:19" ht="17">
@@ -8465,19 +8466,19 @@
         <v>132</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>385</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="F133" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H133" s="15">
         <v>1866</v>
@@ -8501,7 +8502,7 @@
         <v>86</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="134" spans="1:19" ht="17">
@@ -8509,19 +8510,19 @@
         <v>133</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>385</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="F134" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H134" s="15">
         <v>1476</v>
@@ -8545,7 +8546,7 @@
         <v>86</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="135" spans="1:19" ht="17">
@@ -8553,19 +8554,19 @@
         <v>134</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>385</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="F135" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G135" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H135" s="15">
         <v>761</v>
@@ -8589,7 +8590,7 @@
         <v>86</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="136" spans="1:19" ht="17">
@@ -8597,22 +8598,22 @@
         <v>135</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>371</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F136" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H136" s="15">
         <v>913</v>
@@ -8636,7 +8637,7 @@
         <v>74</v>
       </c>
       <c r="S136" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="137" spans="1:19" ht="17">
@@ -8644,22 +8645,22 @@
         <v>136</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>371</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F137" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H137" s="15">
         <v>2050</v>
@@ -8683,7 +8684,7 @@
         <v>74</v>
       </c>
       <c r="S137" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="138" spans="1:19" ht="17">
@@ -8691,19 +8692,19 @@
         <v>137</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E138" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>395</v>
       </c>
       <c r="F138" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H138" s="15">
         <v>6430</v>
@@ -8727,7 +8728,7 @@
         <v>342</v>
       </c>
       <c r="S138" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="139" spans="1:19" ht="17">
@@ -8735,16 +8736,16 @@
         <v>138</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D139" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E139" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="E139" s="7" t="s">
-        <v>401</v>
       </c>
       <c r="F139" s="7" t="s">
         <v>26</v>
@@ -8774,7 +8775,7 @@
         <v>376</v>
       </c>
       <c r="S139" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="140" spans="1:19" ht="17">
@@ -8782,16 +8783,16 @@
         <v>139</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E140" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F140" s="7" t="s">
         <v>26</v>
@@ -8821,7 +8822,7 @@
         <v>376</v>
       </c>
       <c r="S140" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="141" spans="1:19" ht="17">
@@ -8829,16 +8830,16 @@
         <v>140</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E141" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="E141" s="7" t="s">
-        <v>401</v>
       </c>
       <c r="F141" s="7" t="s">
         <v>26</v>
@@ -8868,7 +8869,7 @@
         <v>376</v>
       </c>
       <c r="S141" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="142" spans="1:19" ht="17">
@@ -8876,13 +8877,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F142" s="7" t="s">
         <v>26</v>
@@ -8912,7 +8913,7 @@
         <v>6</v>
       </c>
       <c r="S142" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="143" spans="1:19" ht="17">
@@ -8920,13 +8921,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F143" s="7" t="s">
         <v>26</v>
@@ -8956,7 +8957,7 @@
         <v>6</v>
       </c>
       <c r="S143" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144" spans="1:19" ht="17">
@@ -8964,13 +8965,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>26</v>
@@ -9000,7 +9001,7 @@
         <v>6</v>
       </c>
       <c r="S144" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="145" spans="1:19" ht="17">
@@ -9008,13 +9009,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F145" s="7" t="s">
         <v>26</v>
@@ -9044,7 +9045,7 @@
         <v>6</v>
       </c>
       <c r="S145" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="146" spans="1:19" ht="17">
@@ -9052,13 +9053,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E146" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>26</v>
@@ -9088,7 +9089,7 @@
         <v>6</v>
       </c>
       <c r="S146" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9096,19 +9097,19 @@
         <v>146</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F147" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="G147" s="7" t="s">
         <v>410</v>
-      </c>
-      <c r="G147" s="7" t="s">
-        <v>411</v>
       </c>
       <c r="H147" s="15">
         <v>602</v>
@@ -9129,10 +9130,10 @@
         <v>11</v>
       </c>
       <c r="R147" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S147" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="148" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9140,19 +9141,19 @@
         <v>147</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H148" s="15">
         <v>1121</v>
@@ -9173,10 +9174,10 @@
         <v>11</v>
       </c>
       <c r="R148" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S148" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="149" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9184,19 +9185,19 @@
         <v>148</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G149" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H149" s="15">
         <v>1367</v>
@@ -9217,10 +9218,10 @@
         <v>11</v>
       </c>
       <c r="R149" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S149" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="150" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9228,19 +9229,19 @@
         <v>149</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F150" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G150" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H150" s="15">
         <v>380</v>
@@ -9261,10 +9262,10 @@
         <v>11</v>
       </c>
       <c r="R150" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S150" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="151" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9272,19 +9273,19 @@
         <v>150</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F151" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H151" s="15">
         <v>1246</v>
@@ -9308,7 +9309,7 @@
         <v>6</v>
       </c>
       <c r="S151" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="152" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9316,19 +9317,19 @@
         <v>151</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E152" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F152" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G152" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H152" s="15">
         <v>1370</v>
@@ -9352,7 +9353,7 @@
         <v>6</v>
       </c>
       <c r="S152" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="153" spans="1:19" s="7" customFormat="1" ht="17">
@@ -9360,19 +9361,19 @@
         <v>152</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D153" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F153" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H153" s="15">
         <v>3652</v>
@@ -9396,7 +9397,7 @@
         <v>6</v>
       </c>
       <c r="S153" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update codes and README
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/evaluation_datasets.xlsx
+++ b/Chunk1-Data preparation/evaluation_datasets.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2EF476-562F-1D45-B1BC-CF84CF49F91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E956F-4D11-8D41-8DB9-C2DD5E7F37C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="11" r:id="rId1"/>
@@ -2107,10 +2107,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A4ABD-8CCB-49A1-A4C9-DACBF4835462}">
   <dimension ref="A1:T153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E131" sqref="E131"/>
+      <selection pane="bottomLeft" activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>

</xml_diff>